<commit_message>
final changes before the new version
</commit_message>
<xml_diff>
--- a/xlsx/Template_resources_v2.xlsx
+++ b/xlsx/Template_resources_v2.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofexeteruk-my.sharepoint.com/personal/o_ugur_exeter_ac_uk/Documents/Desktop/rc1.2_ou/metadata-schema/xlsx/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="19" documentId="8_{99403E91-E8F5-414D-961D-BC992CC29E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DC251111-E9FC-4AD1-82E6-B36751046BF8}"/>
+  <xr:revisionPtr revIDLastSave="25" documentId="8_{99403E91-E8F5-414D-961D-BC992CC29E3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9FFC12AF-CB39-4F82-AB12-D4A9F7E7847B}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="14016" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="190">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="191">
   <si>
     <t> </t>
   </si>
@@ -152,12 +152,6 @@
     <t>Rights Ownership </t>
   </si>
   <si>
-    <t>Licence </t>
-  </si>
-  <si>
-    <t>Rights Statement</t>
-  </si>
-  <si>
     <t>Cultural Sensitivity</t>
   </si>
   <si>
@@ -606,6 +600,15 @@
   </si>
   <si>
     <t>Highly sensitive, Medium sensitive, Low sensitive</t>
+  </si>
+  <si>
+    <t>Rights</t>
+  </si>
+  <si>
+    <t>Traditional Knowledge Label</t>
+  </si>
+  <si>
+    <t>Biocultural Label</t>
   </si>
 </sst>
 </file>
@@ -868,6 +871,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1167,10 +1174,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:AQ36"/>
+  <dimension ref="A1:AR36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="J17" sqref="J17"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="Y22" sqref="Y22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1203,16 +1210,17 @@
     <col min="28" max="30" width="26.109375" style="4" customWidth="1"/>
     <col min="31" max="31" width="31.44140625" style="4" customWidth="1"/>
     <col min="32" max="32" width="26.109375" style="4" customWidth="1"/>
-    <col min="33" max="33" width="30.6640625" style="4" customWidth="1"/>
-    <col min="34" max="34" width="32.109375" style="4" customWidth="1"/>
-    <col min="35" max="35" width="20.44140625" style="4" customWidth="1"/>
-    <col min="36" max="36" width="22" style="4" customWidth="1"/>
-    <col min="37" max="37" width="27.5546875" style="4" customWidth="1"/>
-    <col min="38" max="38" width="55.88671875" style="4" customWidth="1"/>
-    <col min="39" max="16384" width="9.109375" style="4"/>
+    <col min="33" max="33" width="33.5546875" style="4" customWidth="1"/>
+    <col min="34" max="34" width="30.6640625" style="4" customWidth="1"/>
+    <col min="35" max="35" width="32.109375" style="4" customWidth="1"/>
+    <col min="36" max="36" width="20.44140625" style="4" customWidth="1"/>
+    <col min="37" max="37" width="22" style="4" customWidth="1"/>
+    <col min="38" max="38" width="27.5546875" style="4" customWidth="1"/>
+    <col min="39" max="39" width="55.88671875" style="4" customWidth="1"/>
+    <col min="40" max="16384" width="9.109375" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1339,9 +1347,12 @@
       <c r="AP1" s="2">
         <v>41</v>
       </c>
-      <c r="AQ1" s="3"/>
+      <c r="AQ1" s="2">
+        <v>42</v>
+      </c>
+      <c r="AR1" s="3"/>
     </row>
-    <row r="2" spans="1:43" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:44" s="7" customFormat="1" ht="23.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1356,7 +1367,7 @@
       <c r="H2" s="26"/>
       <c r="I2" s="27"/>
       <c r="J2" s="26" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="K2" s="26"/>
       <c r="L2" s="26"/>
@@ -1393,20 +1404,21 @@
       <c r="AG2" s="26"/>
       <c r="AH2" s="26"/>
       <c r="AI2" s="26"/>
-      <c r="AJ2" s="27"/>
-      <c r="AK2" s="26" t="s">
+      <c r="AJ2" s="26"/>
+      <c r="AK2" s="27"/>
+      <c r="AL2" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="AL2" s="27"/>
-      <c r="AM2" s="28" t="s">
+      <c r="AM2" s="27"/>
+      <c r="AN2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AN2" s="28"/>
       <c r="AO2" s="28"/>
-      <c r="AP2" s="29"/>
-      <c r="AQ2" s="6"/>
+      <c r="AP2" s="28"/>
+      <c r="AQ2" s="29"/>
+      <c r="AR2" s="6"/>
     </row>
-    <row r="3" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
         <v>9</v>
       </c>
@@ -1438,7 +1450,7 @@
         <v>18</v>
       </c>
       <c r="K3" s="10" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="L3" s="13" t="s">
         <v>19</v>
@@ -1465,7 +1477,7 @@
         <v>26</v>
       </c>
       <c r="T3" s="12" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="U3" s="14" t="s">
         <v>27</v>
@@ -1501,292 +1513,297 @@
         <v>37</v>
       </c>
       <c r="AF3" s="9" t="s">
+        <v>188</v>
+      </c>
+      <c r="AG3" s="10" t="s">
+        <v>189</v>
+      </c>
+      <c r="AH3" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="AI3" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AG3" s="10" t="s">
+      <c r="AJ3" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="AH3" s="9" t="s">
+      <c r="AK3" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="AI3" s="13" t="s">
+      <c r="AL3" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="AJ3" s="13" t="s">
+      <c r="AM3" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="AK3" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="AL3" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="AM3" s="3"/>
       <c r="AN3" s="3"/>
       <c r="AO3" s="3"/>
       <c r="AP3" s="3"/>
       <c r="AQ3" s="3"/>
+      <c r="AR3" s="3"/>
     </row>
-    <row r="4" spans="1:43" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="16" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="16" t="s">
         <v>45</v>
       </c>
-      <c r="B4" s="16" t="s">
+      <c r="D4" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="16" t="s">
+      <c r="E4" s="16" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="F4" s="16" t="s">
         <v>48</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="G4" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="H4" s="16" t="s">
         <v>50</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="I4" s="16" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="16" t="s">
+      <c r="J4" s="17" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="K4" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="J4" s="17" t="s">
+      <c r="L4" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="K4" s="16" t="s">
+      <c r="M4" s="16" t="s">
         <v>55</v>
       </c>
-      <c r="L4" s="16" t="s">
+      <c r="N4" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="M4" s="16" t="s">
+      <c r="O4" s="16" t="s">
+        <v>56</v>
+      </c>
+      <c r="P4" s="16" t="s">
         <v>57</v>
       </c>
-      <c r="N4" s="16" t="s">
+      <c r="Q4" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="O4" s="16" t="s">
-        <v>58</v>
-      </c>
-      <c r="P4" s="16" t="s">
+      <c r="R4" s="16" t="s">
         <v>59</v>
-      </c>
-      <c r="Q4" s="16" t="s">
-        <v>60</v>
-      </c>
-      <c r="R4" s="16" t="s">
-        <v>61</v>
       </c>
       <c r="S4" s="16" t="s">
         <v>0</v>
       </c>
       <c r="T4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="U4" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="V4" s="18" t="s">
         <v>62</v>
       </c>
-      <c r="U4" s="16" t="s">
+      <c r="W4" s="16" t="s">
         <v>63</v>
       </c>
-      <c r="V4" s="18" t="s">
+      <c r="X4" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="W4" s="16" t="s">
+      <c r="Y4" s="16" t="s">
         <v>65</v>
       </c>
-      <c r="X4" s="16" t="s">
+      <c r="Z4" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="Y4" s="16" t="s">
+      <c r="AA4" s="16" t="s">
         <v>67</v>
       </c>
-      <c r="Z4" s="16" t="s">
+      <c r="AB4" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="AA4" s="16" t="s">
+      <c r="AC4" s="16" t="s">
         <v>69</v>
       </c>
-      <c r="AB4" s="16" t="s">
+      <c r="AD4" s="16" t="s">
         <v>70</v>
       </c>
-      <c r="AC4" s="16" t="s">
+      <c r="AE4" s="16" t="s">
         <v>71</v>
       </c>
-      <c r="AD4" s="16" t="s">
+      <c r="AF4" s="16" t="s">
         <v>72</v>
       </c>
-      <c r="AE4" s="16" t="s">
+      <c r="AG4" s="17" t="s">
         <v>73</v>
       </c>
-      <c r="AF4" s="16" t="s">
+      <c r="AH4" s="17"/>
+      <c r="AI4" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="AG4" s="17" t="s">
+      <c r="AJ4" s="16" t="s">
         <v>75</v>
       </c>
-      <c r="AH4" s="16" t="s">
+      <c r="AK4" s="16" t="s">
         <v>76</v>
       </c>
-      <c r="AI4" s="16" t="s">
+      <c r="AL4" s="16" t="s">
         <v>77</v>
       </c>
-      <c r="AJ4" s="16" t="s">
+      <c r="AM4" s="16" t="s">
         <v>78</v>
       </c>
-      <c r="AK4" s="16" t="s">
-        <v>79</v>
-      </c>
-      <c r="AL4" s="16" t="s">
-        <v>80</v>
-      </c>
-      <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="3"/>
+      <c r="AR4" s="3"/>
     </row>
-    <row r="5" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A5" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>80</v>
+      </c>
+      <c r="C5" s="19" t="s">
         <v>81</v>
       </c>
-      <c r="B5" s="16" t="s">
+      <c r="D5" s="16" t="s">
         <v>82</v>
       </c>
-      <c r="C5" s="19" t="s">
+      <c r="E5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="G5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="H5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="I5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="J5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="K5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="L5" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="M5" s="16" t="s">
+        <v>83</v>
+      </c>
+      <c r="N5" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="E5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="F5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="G5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="H5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="I5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="J5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="K5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="L5" s="16" t="s">
+      <c r="O5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="P5" s="16" t="s">
         <v>85</v>
       </c>
-      <c r="M5" s="16" t="s">
-        <v>85</v>
-      </c>
-      <c r="N5" s="16" t="s">
+      <c r="Q5" s="16" t="s">
         <v>86</v>
       </c>
-      <c r="O5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="P5" s="16" t="s">
+      <c r="R5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="S5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="T5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="U5" s="16" t="s">
         <v>87</v>
       </c>
-      <c r="Q5" s="16" t="s">
+      <c r="V5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="W5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="X5" s="16" t="s">
         <v>88</v>
       </c>
-      <c r="R5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="S5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="T5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="U5" s="16" t="s">
+      <c r="Y5" s="16" t="s">
         <v>89</v>
       </c>
-      <c r="V5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="W5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="X5" s="16" t="s">
+      <c r="Z5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AA5" s="19" t="s">
+        <v>81</v>
+      </c>
+      <c r="AB5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AC5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AD5" s="16" t="s">
+        <v>87</v>
+      </c>
+      <c r="AE5" s="16" t="s">
         <v>90</v>
       </c>
-      <c r="Y5" s="16" t="s">
+      <c r="AF5" s="16" t="s">
         <v>91</v>
       </c>
-      <c r="Z5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="AA5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="AB5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AC5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AD5" s="16" t="s">
-        <v>89</v>
-      </c>
-      <c r="AE5" s="16" t="s">
+      <c r="AG5" s="16" t="s">
         <v>92</v>
       </c>
-      <c r="AF5" s="16" t="s">
+      <c r="AH5" s="16"/>
+      <c r="AI5" s="16" t="s">
         <v>93</v>
       </c>
-      <c r="AG5" s="16" t="s">
+      <c r="AJ5" s="16" t="s">
         <v>94</v>
       </c>
-      <c r="AH5" s="16" t="s">
-        <v>95</v>
-      </c>
-      <c r="AI5" s="16" t="s">
-        <v>96</v>
-      </c>
-      <c r="AJ5" s="19" t="s">
-        <v>83</v>
-      </c>
-      <c r="AK5" s="16" t="s">
-        <v>92</v>
+      <c r="AK5" s="19" t="s">
+        <v>81</v>
       </c>
       <c r="AL5" s="16" t="s">
-        <v>92</v>
-      </c>
-      <c r="AM5" s="3"/>
+        <v>90</v>
+      </c>
+      <c r="AM5" s="16" t="s">
+        <v>90</v>
+      </c>
       <c r="AN5" s="3"/>
       <c r="AO5" s="3"/>
       <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
+      <c r="AR5" s="3"/>
     </row>
-    <row r="6" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A6" s="8" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B6" s="16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C6" s="20" t="s">
         <v>0</v>
       </c>
       <c r="D6" s="16" t="s">
+        <v>97</v>
+      </c>
+      <c r="E6" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="F6" s="16" t="s">
         <v>99</v>
-      </c>
-      <c r="E6" s="16" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="16" t="s">
-        <v>101</v>
       </c>
       <c r="G6" s="20" t="s">
         <v>0</v>
@@ -1795,46 +1812,46 @@
         <v>0</v>
       </c>
       <c r="I6" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="J6" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="K6" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="L6" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="J6" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="K6" s="16" t="s">
-        <v>103</v>
-      </c>
-      <c r="L6" s="16" t="s">
-        <v>104</v>
-      </c>
       <c r="M6" s="16" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="N6" s="20" t="s">
         <v>0</v>
       </c>
       <c r="O6" s="16" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="P6" s="20" t="s">
         <v>0</v>
       </c>
       <c r="Q6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="R6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="S6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="U6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="V6" s="16" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="W6" s="20" t="s">
         <v>0</v>
@@ -1852,7 +1869,7 @@
         <v>0</v>
       </c>
       <c r="AB6" s="16" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="AC6" s="20" t="s">
         <v>0</v>
@@ -1861,298 +1878,301 @@
         <v>0</v>
       </c>
       <c r="AE6" s="16" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="AF6" s="16" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="AG6" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="AH6" s="20" t="s">
-        <v>0</v>
-      </c>
+      <c r="AH6" s="16"/>
       <c r="AI6" s="20" t="s">
         <v>0</v>
       </c>
       <c r="AJ6" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="AK6" s="16" t="s">
-        <v>110</v>
+      <c r="AK6" s="20" t="s">
+        <v>0</v>
       </c>
       <c r="AL6" s="16" t="s">
-        <v>111</v>
-      </c>
-      <c r="AM6" s="3"/>
+        <v>108</v>
+      </c>
+      <c r="AM6" s="16" t="s">
+        <v>109</v>
+      </c>
       <c r="AN6" s="3"/>
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3"/>
+      <c r="AR6" s="3"/>
     </row>
-    <row r="7" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A7" s="8" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="C7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="D7" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="C7" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="D7" s="16" t="s">
-        <v>115</v>
-      </c>
       <c r="E7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="F7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="G7" s="16" t="s">
+        <v>111</v>
+      </c>
+      <c r="H7" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="I7" s="16" t="s">
+        <v>112</v>
+      </c>
+      <c r="J7" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="K7" s="16" t="s">
         <v>113</v>
       </c>
-      <c r="H7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="I7" s="16" t="s">
-        <v>114</v>
-      </c>
-      <c r="J7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="K7" s="16" t="s">
-        <v>115</v>
-      </c>
       <c r="L7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="M7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="N7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="O7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="P7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Q7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="R7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="S7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="T7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="U7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="V7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="W7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="X7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Y7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="Z7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AA7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AB7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AC7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AD7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AE7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AF7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AG7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AH7" s="16" t="s">
-        <v>115</v>
-      </c>
+        <v>113</v>
+      </c>
+      <c r="AH7" s="16"/>
       <c r="AI7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AJ7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AK7" s="16" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="AL7" s="16" t="s">
-        <v>115</v>
-      </c>
-      <c r="AM7" s="3"/>
+        <v>113</v>
+      </c>
+      <c r="AM7" s="16" t="s">
+        <v>113</v>
+      </c>
       <c r="AN7" s="3"/>
       <c r="AO7" s="3"/>
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
+      <c r="AR7" s="3"/>
     </row>
-    <row r="8" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A8" s="8" t="s">
+        <v>114</v>
+      </c>
+      <c r="B8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="C8" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="B8" s="16" t="s">
+      <c r="D8" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="C8" s="16" t="s">
+      <c r="E8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="F8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="G8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="H8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="I8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="J8" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="K8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="L8" s="16" t="s">
         <v>119</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="M8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="N8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="O8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="P8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="Q8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="R8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="S8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="T8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="U8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="V8" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="W8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="X8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="Z8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AA8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AB8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="AC8" s="21" t="s">
+        <v>118</v>
+      </c>
+      <c r="AD8" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="AE8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AF8" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="AG8" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="AH8" s="16"/>
+      <c r="AI8" s="16" t="s">
         <v>117</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="AJ8" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="AK8" s="16" t="s">
+        <v>122</v>
+      </c>
+      <c r="AL8" s="21" t="s">
         <v>118</v>
       </c>
-      <c r="G8" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="H8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="I8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="J8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="K8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="L8" s="16" t="s">
-        <v>121</v>
-      </c>
-      <c r="M8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="N8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="O8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="P8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="Q8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="R8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="S8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="T8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="U8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="V8" s="18" t="s">
-        <v>122</v>
-      </c>
-      <c r="W8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="X8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="Y8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="Z8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="AA8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="AB8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="AC8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="AD8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="AE8" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="AF8" s="16" t="s">
-        <v>117</v>
-      </c>
-      <c r="AG8" s="16" t="s">
-        <v>122</v>
-      </c>
-      <c r="AH8" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="AI8" s="16" t="s">
-        <v>123</v>
-      </c>
-      <c r="AJ8" s="16" t="s">
-        <v>124</v>
-      </c>
-      <c r="AK8" s="21" t="s">
-        <v>120</v>
-      </c>
-      <c r="AL8" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="AM8" s="3"/>
+      <c r="AM8" s="16" t="s">
+        <v>116</v>
+      </c>
       <c r="AN8" s="3"/>
       <c r="AO8" s="3"/>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3"/>
+      <c r="AR8" s="3"/>
     </row>
-    <row r="9" spans="1:43" ht="45" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:44" ht="45" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="8" t="s">
+        <v>123</v>
+      </c>
+      <c r="B9" s="16" t="s">
+        <v>124</v>
+      </c>
+      <c r="C9" s="16" t="s">
         <v>125</v>
       </c>
-      <c r="B9" s="16" t="s">
+      <c r="D9" s="16" t="s">
         <v>126</v>
       </c>
-      <c r="C9" s="16" t="s">
+      <c r="E9" s="16" t="s">
         <v>127</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="F9" s="16" t="s">
         <v>128</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="G9" s="16" t="s">
         <v>129</v>
-      </c>
-      <c r="F9" s="16" t="s">
-        <v>130</v>
-      </c>
-      <c r="G9" s="16" t="s">
-        <v>131</v>
       </c>
       <c r="H9" s="16" t="s">
         <v>0</v>
@@ -2161,119 +2181,120 @@
         <v>0</v>
       </c>
       <c r="J9" s="16" t="s">
+        <v>130</v>
+      </c>
+      <c r="K9" s="16" t="s">
+        <v>131</v>
+      </c>
+      <c r="L9" s="16" t="s">
         <v>132</v>
       </c>
-      <c r="K9" s="16" t="s">
+      <c r="M9" s="16" t="s">
         <v>133</v>
       </c>
-      <c r="L9" s="16" t="s">
+      <c r="N9" s="16" t="s">
         <v>134</v>
       </c>
-      <c r="M9" s="16" t="s">
-        <v>135</v>
-      </c>
-      <c r="N9" s="16" t="s">
-        <v>136</v>
-      </c>
       <c r="O9" s="16" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="P9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="Q9" s="16" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="R9" s="16" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="S9" s="16" t="s">
         <v>0</v>
       </c>
       <c r="T9" s="16" t="s">
+        <v>137</v>
+      </c>
+      <c r="U9" s="16" t="s">
+        <v>138</v>
+      </c>
+      <c r="V9" s="18" t="s">
         <v>139</v>
       </c>
-      <c r="U9" s="16" t="s">
+      <c r="W9" s="16" t="s">
         <v>140</v>
       </c>
-      <c r="V9" s="18" t="s">
+      <c r="X9" s="16" t="s">
         <v>141</v>
       </c>
-      <c r="W9" s="16" t="s">
+      <c r="Y9" s="16" t="s">
         <v>142</v>
       </c>
-      <c r="X9" s="16" t="s">
+      <c r="Z9" s="16" t="s">
         <v>143</v>
       </c>
-      <c r="Y9" s="16" t="s">
+      <c r="AA9" s="16" t="s">
         <v>144</v>
       </c>
-      <c r="Z9" s="16" t="s">
+      <c r="AB9" s="16" t="s">
         <v>145</v>
       </c>
-      <c r="AA9" s="16" t="s">
+      <c r="AC9" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AD9" s="16" t="s">
+        <v>145</v>
+      </c>
+      <c r="AE9" s="16" t="s">
         <v>146</v>
       </c>
-      <c r="AB9" s="16" t="s">
+      <c r="AF9" s="16" t="s">
         <v>147</v>
       </c>
-      <c r="AC9" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="AD9" s="16" t="s">
-        <v>147</v>
-      </c>
-      <c r="AE9" s="16" t="s">
+      <c r="AG9" s="16" t="s">
         <v>148</v>
       </c>
-      <c r="AF9" s="16" t="s">
+      <c r="AH9" s="16"/>
+      <c r="AI9" s="16" t="s">
         <v>149</v>
       </c>
-      <c r="AG9" s="16" t="s">
+      <c r="AJ9" s="16" t="s">
         <v>150</v>
       </c>
-      <c r="AH9" s="16" t="s">
+      <c r="AK9" s="16" t="s">
         <v>151</v>
       </c>
-      <c r="AI9" s="16" t="s">
+      <c r="AL9" s="16" t="s">
         <v>152</v>
       </c>
-      <c r="AJ9" s="16" t="s">
+      <c r="AM9" s="16" t="s">
         <v>153</v>
       </c>
-      <c r="AK9" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="AL9" s="16" t="s">
-        <v>155</v>
-      </c>
-      <c r="AM9" s="3"/>
       <c r="AN9" s="3"/>
       <c r="AO9" s="3"/>
       <c r="AP9" s="3"/>
       <c r="AQ9" s="3"/>
+      <c r="AR9" s="3"/>
     </row>
-    <row r="10" spans="1:43" ht="39" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:44" ht="39" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="8" t="s">
+        <v>154</v>
+      </c>
+      <c r="B10" s="16" t="s">
+        <v>155</v>
+      </c>
+      <c r="C10" s="16" t="s">
         <v>156</v>
       </c>
-      <c r="B10" s="16" t="s">
+      <c r="D10" s="16" t="s">
         <v>157</v>
       </c>
-      <c r="C10" s="16" t="s">
+      <c r="E10" s="16" t="s">
         <v>158</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="F10" s="16" t="s">
         <v>159</v>
       </c>
-      <c r="E10" s="16" t="s">
+      <c r="G10" s="16" t="s">
         <v>160</v>
-      </c>
-      <c r="F10" s="16" t="s">
-        <v>161</v>
-      </c>
-      <c r="G10" s="16" t="s">
-        <v>162</v>
       </c>
       <c r="H10" s="16" t="s">
         <v>0</v>
@@ -2282,99 +2303,100 @@
         <v>0</v>
       </c>
       <c r="J10" s="16" t="s">
+        <v>161</v>
+      </c>
+      <c r="K10" s="16" t="s">
+        <v>162</v>
+      </c>
+      <c r="L10" s="16" t="s">
         <v>163</v>
       </c>
-      <c r="K10" s="16" t="s">
+      <c r="M10" s="16" t="s">
+        <v>163</v>
+      </c>
+      <c r="N10" s="16" t="s">
         <v>164</v>
       </c>
-      <c r="L10" s="16" t="s">
+      <c r="O10" s="16" t="s">
         <v>165</v>
-      </c>
-      <c r="M10" s="16" t="s">
-        <v>165</v>
-      </c>
-      <c r="N10" s="16" t="s">
-        <v>166</v>
-      </c>
-      <c r="O10" s="16" t="s">
-        <v>167</v>
       </c>
       <c r="P10" s="16" t="s">
         <v>0</v>
       </c>
       <c r="Q10" s="16" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="R10" s="16" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="S10" s="16" t="s">
         <v>0</v>
       </c>
       <c r="T10" s="16" t="s">
+        <v>168</v>
+      </c>
+      <c r="U10" s="16" t="s">
+        <v>169</v>
+      </c>
+      <c r="V10" s="18" t="s">
         <v>170</v>
       </c>
-      <c r="U10" s="16" t="s">
+      <c r="W10" s="16" t="s">
         <v>171</v>
       </c>
-      <c r="V10" s="18" t="s">
+      <c r="X10" s="16" t="s">
         <v>172</v>
       </c>
-      <c r="W10" s="16" t="s">
+      <c r="Y10" s="16" t="s">
         <v>173</v>
       </c>
-      <c r="X10" s="16" t="s">
+      <c r="Z10" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="Y10" s="16" t="s">
+      <c r="AA10" s="16" t="s">
         <v>175</v>
       </c>
-      <c r="Z10" s="16" t="s">
+      <c r="AB10" s="16" t="s">
         <v>176</v>
       </c>
-      <c r="AA10" s="16" t="s">
+      <c r="AC10" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD10" s="16" t="s">
+        <v>176</v>
+      </c>
+      <c r="AE10" s="16" t="s">
         <v>177</v>
       </c>
-      <c r="AB10" s="16" t="s">
+      <c r="AF10" s="16" t="s">
         <v>178</v>
       </c>
-      <c r="AC10" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="AD10" s="16" t="s">
-        <v>178</v>
-      </c>
-      <c r="AE10" s="16" t="s">
+      <c r="AG10" s="16" t="s">
         <v>179</v>
       </c>
-      <c r="AF10" s="16" t="s">
+      <c r="AH10" s="16"/>
+      <c r="AI10" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="AJ10" s="16" t="s">
         <v>180</v>
       </c>
-      <c r="AG10" s="16" t="s">
+      <c r="AK10" s="16" t="s">
         <v>181</v>
       </c>
-      <c r="AH10" s="22" t="s">
-        <v>189</v>
-      </c>
-      <c r="AI10" s="16" t="s">
+      <c r="AL10" s="16" t="s">
         <v>182</v>
       </c>
-      <c r="AJ10" s="16" t="s">
+      <c r="AM10" s="16" t="s">
         <v>183</v>
       </c>
-      <c r="AK10" s="16" t="s">
-        <v>184</v>
-      </c>
-      <c r="AL10" s="16" t="s">
-        <v>185</v>
-      </c>
-      <c r="AM10" s="3"/>
       <c r="AN10" s="3"/>
       <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
+      <c r="AR10" s="3"/>
     </row>
-    <row r="11" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A11" s="23"/>
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
@@ -2408,18 +2430,19 @@
       <c r="AE11" s="23"/>
       <c r="AF11" s="23"/>
       <c r="AG11" s="24"/>
-      <c r="AH11" s="23"/>
+      <c r="AH11" s="24"/>
       <c r="AI11" s="23"/>
       <c r="AJ11" s="23"/>
       <c r="AK11" s="23"/>
       <c r="AL11" s="23"/>
-      <c r="AM11" s="3"/>
+      <c r="AM11" s="23"/>
       <c r="AN11" s="3"/>
       <c r="AO11" s="3"/>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
+      <c r="AR11" s="3"/>
     </row>
-    <row r="12" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A12" s="23"/>
       <c r="B12" s="23"/>
       <c r="C12" s="23"/>
@@ -2453,7 +2476,7 @@
       <c r="AE12" s="23"/>
       <c r="AF12" s="23"/>
       <c r="AG12" s="24"/>
-      <c r="AH12" s="23"/>
+      <c r="AH12" s="24"/>
       <c r="AI12" s="23"/>
       <c r="AJ12" s="23"/>
       <c r="AK12" s="23"/>
@@ -2462,9 +2485,10 @@
       <c r="AN12" s="23"/>
       <c r="AO12" s="23"/>
       <c r="AP12" s="23"/>
-      <c r="AQ12" s="3"/>
+      <c r="AQ12" s="23"/>
+      <c r="AR12" s="3"/>
     </row>
-    <row r="13" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A13" s="23"/>
       <c r="B13" s="23"/>
       <c r="C13" s="23"/>
@@ -2498,7 +2522,7 @@
       <c r="AE13" s="23"/>
       <c r="AF13" s="23"/>
       <c r="AG13" s="24"/>
-      <c r="AH13" s="23"/>
+      <c r="AH13" s="24"/>
       <c r="AI13" s="23"/>
       <c r="AJ13" s="23"/>
       <c r="AK13" s="23"/>
@@ -2507,9 +2531,10 @@
       <c r="AN13" s="23"/>
       <c r="AO13" s="23"/>
       <c r="AP13" s="23"/>
-      <c r="AQ13" s="3"/>
+      <c r="AQ13" s="23"/>
+      <c r="AR13" s="3"/>
     </row>
-    <row r="14" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A14" s="23"/>
       <c r="B14" s="23"/>
       <c r="C14" s="23"/>
@@ -2543,7 +2568,7 @@
       <c r="AE14" s="23"/>
       <c r="AF14" s="23"/>
       <c r="AG14" s="24"/>
-      <c r="AH14" s="23"/>
+      <c r="AH14" s="24"/>
       <c r="AI14" s="23"/>
       <c r="AJ14" s="23"/>
       <c r="AK14" s="23"/>
@@ -2552,9 +2577,10 @@
       <c r="AN14" s="23"/>
       <c r="AO14" s="23"/>
       <c r="AP14" s="23"/>
-      <c r="AQ14" s="3"/>
+      <c r="AQ14" s="23"/>
+      <c r="AR14" s="3"/>
     </row>
-    <row r="15" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A15" s="23"/>
       <c r="B15" s="23"/>
       <c r="C15" s="23"/>
@@ -2588,18 +2614,19 @@
       <c r="AE15" s="23"/>
       <c r="AF15" s="23"/>
       <c r="AG15" s="24"/>
-      <c r="AH15" s="23"/>
+      <c r="AH15" s="24"/>
       <c r="AI15" s="23"/>
       <c r="AJ15" s="23"/>
       <c r="AK15" s="23"/>
       <c r="AL15" s="23"/>
-      <c r="AM15" s="3"/>
+      <c r="AM15" s="23"/>
       <c r="AN15" s="3"/>
       <c r="AO15" s="3"/>
       <c r="AP15" s="3"/>
       <c r="AQ15" s="3"/>
+      <c r="AR15" s="3"/>
     </row>
-    <row r="16" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A16" s="23"/>
       <c r="B16" s="23"/>
       <c r="C16" s="23"/>
@@ -2633,18 +2660,19 @@
       <c r="AE16" s="23"/>
       <c r="AF16" s="23"/>
       <c r="AG16" s="24"/>
-      <c r="AH16" s="23"/>
+      <c r="AH16" s="24"/>
       <c r="AI16" s="23"/>
       <c r="AJ16" s="23"/>
       <c r="AK16" s="23"/>
       <c r="AL16" s="23"/>
-      <c r="AM16" s="3"/>
+      <c r="AM16" s="23"/>
       <c r="AN16" s="3"/>
       <c r="AO16" s="3"/>
       <c r="AP16" s="3"/>
       <c r="AQ16" s="3"/>
+      <c r="AR16" s="3"/>
     </row>
-    <row r="17" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A17" s="23"/>
       <c r="B17" s="23"/>
       <c r="C17" s="23"/>
@@ -2678,18 +2706,19 @@
       <c r="AE17" s="23"/>
       <c r="AF17" s="23"/>
       <c r="AG17" s="24"/>
-      <c r="AH17" s="23"/>
+      <c r="AH17" s="24"/>
       <c r="AI17" s="23"/>
       <c r="AJ17" s="23"/>
       <c r="AK17" s="23"/>
       <c r="AL17" s="23"/>
-      <c r="AM17" s="3"/>
+      <c r="AM17" s="23"/>
       <c r="AN17" s="3"/>
       <c r="AO17" s="3"/>
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
+      <c r="AR17" s="3"/>
     </row>
-    <row r="18" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A18" s="23"/>
       <c r="B18" s="23"/>
       <c r="C18" s="23"/>
@@ -2723,18 +2752,19 @@
       <c r="AE18" s="23"/>
       <c r="AF18" s="23"/>
       <c r="AG18" s="24"/>
-      <c r="AH18" s="23"/>
+      <c r="AH18" s="24"/>
       <c r="AI18" s="23"/>
       <c r="AJ18" s="23"/>
       <c r="AK18" s="23"/>
       <c r="AL18" s="23"/>
-      <c r="AM18" s="3"/>
+      <c r="AM18" s="23"/>
       <c r="AN18" s="3"/>
       <c r="AO18" s="3"/>
       <c r="AP18" s="3"/>
       <c r="AQ18" s="3"/>
+      <c r="AR18" s="3"/>
     </row>
-    <row r="19" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A19" s="23"/>
       <c r="B19" s="23"/>
       <c r="C19" s="23"/>
@@ -2768,18 +2798,19 @@
       <c r="AE19" s="23"/>
       <c r="AF19" s="23"/>
       <c r="AG19" s="24"/>
-      <c r="AH19" s="23"/>
+      <c r="AH19" s="24"/>
       <c r="AI19" s="23"/>
       <c r="AJ19" s="23"/>
       <c r="AK19" s="23"/>
       <c r="AL19" s="23"/>
-      <c r="AM19" s="3"/>
+      <c r="AM19" s="23"/>
       <c r="AN19" s="3"/>
       <c r="AO19" s="3"/>
       <c r="AP19" s="3"/>
       <c r="AQ19" s="3"/>
+      <c r="AR19" s="3"/>
     </row>
-    <row r="20" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A20" s="23"/>
       <c r="B20" s="23"/>
       <c r="C20" s="23"/>
@@ -2813,18 +2844,19 @@
       <c r="AE20" s="23"/>
       <c r="AF20" s="23"/>
       <c r="AG20" s="24"/>
-      <c r="AH20" s="23"/>
+      <c r="AH20" s="24"/>
       <c r="AI20" s="23"/>
       <c r="AJ20" s="23"/>
       <c r="AK20" s="23"/>
       <c r="AL20" s="23"/>
-      <c r="AM20" s="3"/>
+      <c r="AM20" s="23"/>
       <c r="AN20" s="3"/>
       <c r="AO20" s="3"/>
       <c r="AP20" s="3"/>
       <c r="AQ20" s="3"/>
+      <c r="AR20" s="3"/>
     </row>
-    <row r="21" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A21" s="23"/>
       <c r="B21" s="23"/>
       <c r="C21" s="23"/>
@@ -2858,7 +2890,7 @@
       <c r="AE21" s="3"/>
       <c r="AF21" s="3"/>
       <c r="AG21" s="25"/>
-      <c r="AH21" s="3"/>
+      <c r="AH21" s="25"/>
       <c r="AI21" s="3"/>
       <c r="AJ21" s="3"/>
       <c r="AK21" s="3"/>
@@ -2868,8 +2900,9 @@
       <c r="AO21" s="3"/>
       <c r="AP21" s="3"/>
       <c r="AQ21" s="3"/>
+      <c r="AR21" s="3"/>
     </row>
-    <row r="22" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A22" s="23"/>
       <c r="B22" s="23"/>
       <c r="C22" s="23"/>
@@ -2913,8 +2946,9 @@
       <c r="AO22" s="3"/>
       <c r="AP22" s="3"/>
       <c r="AQ22" s="3"/>
+      <c r="AR22" s="3"/>
     </row>
-    <row r="23" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A23" s="23"/>
       <c r="B23" s="23"/>
       <c r="C23" s="23"/>
@@ -2953,13 +2987,14 @@
       <c r="AJ23" s="23"/>
       <c r="AK23" s="23"/>
       <c r="AL23" s="23"/>
-      <c r="AM23" s="3"/>
+      <c r="AM23" s="23"/>
       <c r="AN23" s="3"/>
       <c r="AO23" s="3"/>
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
+      <c r="AR23" s="3"/>
     </row>
-    <row r="24" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -3003,8 +3038,9 @@
       <c r="AO24" s="3"/>
       <c r="AP24" s="3"/>
       <c r="AQ24" s="3"/>
+      <c r="AR24" s="3"/>
     </row>
-    <row r="25" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A25" s="3"/>
       <c r="B25" s="3"/>
       <c r="C25" s="3"/>
@@ -3048,8 +3084,9 @@
       <c r="AO25" s="3"/>
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3"/>
+      <c r="AR25" s="3"/>
     </row>
-    <row r="26" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A26" s="3"/>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
@@ -3093,8 +3130,9 @@
       <c r="AO26" s="3"/>
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3"/>
+      <c r="AR26" s="3"/>
     </row>
-    <row r="27" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
       <c r="C27" s="3"/>
@@ -3138,8 +3176,9 @@
       <c r="AO27" s="3"/>
       <c r="AP27" s="3"/>
       <c r="AQ27" s="3"/>
+      <c r="AR27" s="3"/>
     </row>
-    <row r="28" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A28" s="3"/>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
@@ -3183,8 +3222,9 @@
       <c r="AO28" s="3"/>
       <c r="AP28" s="3"/>
       <c r="AQ28" s="3"/>
+      <c r="AR28" s="3"/>
     </row>
-    <row r="29" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A29" s="3"/>
       <c r="B29" s="3"/>
       <c r="C29" s="3"/>
@@ -3228,8 +3268,9 @@
       <c r="AO29" s="3"/>
       <c r="AP29" s="3"/>
       <c r="AQ29" s="3"/>
+      <c r="AR29" s="3"/>
     </row>
-    <row r="30" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A30" s="3"/>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -3273,8 +3314,9 @@
       <c r="AO30" s="3"/>
       <c r="AP30" s="3"/>
       <c r="AQ30" s="3"/>
+      <c r="AR30" s="3"/>
     </row>
-    <row r="31" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A31" s="3"/>
       <c r="B31" s="3"/>
       <c r="C31" s="3"/>
@@ -3318,8 +3360,9 @@
       <c r="AO31" s="3"/>
       <c r="AP31" s="3"/>
       <c r="AQ31" s="3"/>
+      <c r="AR31" s="3"/>
     </row>
-    <row r="32" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -3363,8 +3406,9 @@
       <c r="AO32" s="3"/>
       <c r="AP32" s="3"/>
       <c r="AQ32" s="3"/>
+      <c r="AR32" s="3"/>
     </row>
-    <row r="33" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A33" s="3"/>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -3408,8 +3452,9 @@
       <c r="AO33" s="3"/>
       <c r="AP33" s="3"/>
       <c r="AQ33" s="3"/>
+      <c r="AR33" s="3"/>
     </row>
-    <row r="34" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
@@ -3453,8 +3498,9 @@
       <c r="AO34" s="3"/>
       <c r="AP34" s="3"/>
       <c r="AQ34" s="3"/>
+      <c r="AR34" s="3"/>
     </row>
-    <row r="35" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A35" s="3"/>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
@@ -3498,8 +3544,9 @@
       <c r="AO35" s="3"/>
       <c r="AP35" s="3"/>
       <c r="AQ35" s="3"/>
+      <c r="AR35" s="3"/>
     </row>
-    <row r="36" spans="1:43" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:44" x14ac:dyDescent="0.3">
       <c r="A36" s="3"/>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -3543,6 +3590,7 @@
       <c r="AO36" s="3"/>
       <c r="AP36" s="3"/>
       <c r="AQ36" s="3"/>
+      <c r="AR36" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3551,6 +3599,31 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Relating_x0020_to xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
+    <Templatereturned xmlns="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2" xsi:nil="true"/>
+    <TaxCatchAll xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <Where_x0020_in_x0020_the_x0020_world_x0020_this_x0020_relates xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100892B5F8BA23C904D8BA7C5AD24010DAA" ma:contentTypeVersion="24" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="d7faeb39acc7c50f6481fd70bd029784">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2" xmlns:ns3="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9591e146543a5f77023cb0f7fdff1ce3" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -3885,32 +3958,27 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB66EA13-ACFC-447A-9B90-3F69243421C8}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Relating_x0020_to xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
-    <Templatereturned xmlns="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2" xsi:nil="true"/>
-    <TaxCatchAll xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <Where_x0020_in_x0020_the_x0020_world_x0020_this_x0020_relates xmlns="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-    <_ip_UnifiedCompliancePolicyProperties xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F2198-9ACF-479A-AEB4-8C7C16E6AF72}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e"/>
+    <ds:schemaRef ds:uri="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{71D1BFB7-CE0C-410A-B401-65160B572881}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3928,24 +3996,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB66EA13-ACFC-447A-9B90-3F69243421C8}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A97F2198-9ACF-479A-AEB4-8C7C16E6AF72}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="c1e9efdf-70dd-4c9c-a5bf-775c91aa858e"/>
-    <ds:schemaRef ds:uri="e195f771-0eb3-4b04-a01a-4bda1f0b8ab2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>